<commit_message>
need to be maintained
</commit_message>
<xml_diff>
--- a/weather_data.xlsx
+++ b/weather_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1123,6 +1123,676 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2022030211</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>东风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2022030210</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>东北风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2022030209</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>东风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2022030208</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>东风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2022030207</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>东北风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2022030206</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>东南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2022030205</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>东风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2022030204</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2022030203</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2022030202</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>东风0级</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2022030201</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>东风0级</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2022030200</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>东北风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2022030223</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>南风0级</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2022030222</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>东北风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2022030221</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>东风0级</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2022030220</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>北风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2022030219</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>东北风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2022030218</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>西南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2022030217</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>西南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2022030216</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2022030215</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2022030214</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>西风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2022030213</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>西南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2022030212</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>西南风1级</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2022030211</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>东南风1级</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>